<commit_message>
add optimizing ans. see .json.
</commit_message>
<xml_diff>
--- a/tsp结果表头.xlsx
+++ b/tsp结果表头.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/naiquh/box.nju/Seafile/teaching/2025离散优化算法/2025-课件-离散优化算法/copt_gurobi_cplex/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NJU\Projects\TSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8848128C-813A-6544-9D26-AD74A57620F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA384929-A48F-4B64-BD92-131F257435A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="4800" windowWidth="28240" windowHeight="17440" xr2:uid="{1F621E1B-0013-FB40-BA1E-B470E5CCCC83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F621E1B-0013-FB40-BA1E-B470E5CCCC83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>算例</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,15 +39,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>u724</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>u1060</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>…</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -97,10 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>subtour elimination</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>copt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,15 +101,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(说明采用了什么高级功能，比如xx callback）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CPU型号主频</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Apple M4</t>
+    <t>1. Callback: 只有找到合法子环，才添加lazy constraint把该子环排除；放弃在硬约束中排除所有子环
+2. 求最短子环的函数不会找到对称子环，以破解对称性
+3.在Gurobi求解之前使用最近邻算法生成初始可行路径，并设置为初始解
+4.参数调优：
+model.setParam("MIPFocus", 1)
+            model.setParam("ImproveStartTime", 5)
+            model.setParam("ImproveStartNodes", 100)
+            model.setParam("Cuts", 1)
+            model.setParam("Heuristics", 0.8)
+            model.setParam("Presolve", 1)
+            model.setParam("Threads", 8)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11th Gen Intel(R) Core(TM) i5-1155G7 @ 2.50GHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Subtour Elimination Formulation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. Callback: 只有找到合法子环，才添加lazy constraint把该子环排除；放弃在硬约束中排除所有子环
+2. 参数调优：
+model.setParam(COPT.Param.HeurLevel, 3)
+        model.setParam(COPT.Param.Threads, 8)
+        model.setParam(COPT.Param.Presolve, 2)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -196,12 +197,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,16 +523,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9902200E-5C89-164B-9530-850F7BA4D82E}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="3" max="4" width="18.5" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="21.1640625" customWidth="1"/>
-    <col min="8" max="9" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
+    <col min="4" max="4" width="42.08984375" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" customWidth="1"/>
+    <col min="8" max="9" width="15.6328125" customWidth="1"/>
+    <col min="10" max="10" width="40.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -536,85 +542,223 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" ht="234">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E2">
         <v>600</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
+      <c r="F2">
+        <v>48834</v>
+      </c>
+      <c r="G2">
+        <v>48910</v>
+      </c>
+      <c r="H2">
+        <v>0.15538744632999299</v>
+      </c>
+      <c r="I2">
+        <v>600.04800009727398</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" ht="127.2" customHeight="1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
       <c r="E3">
         <v>600</v>
       </c>
+      <c r="F3">
+        <v>47113</v>
+      </c>
+      <c r="G3">
+        <v>47113</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>32.058999999999997</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" ht="234">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>600</v>
+      </c>
+      <c r="F4">
+        <v>6771</v>
+      </c>
+      <c r="G4">
+        <v>6773</v>
+      </c>
+      <c r="H4">
+        <v>2.9529012254540001E-2</v>
+      </c>
+      <c r="I4">
+        <v>600.03299999237004</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" ht="109.2">
       <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5">
+        <v>600</v>
+      </c>
+      <c r="F5">
+        <v>6685</v>
+      </c>
+      <c r="G5">
+        <v>6685</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>26.873998641966999</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="234">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>600</v>
+      </c>
+      <c r="F6">
+        <v>214023</v>
+      </c>
+      <c r="G6">
+        <v>260179</v>
+      </c>
+      <c r="H6">
+        <v>17.74009431967</v>
+      </c>
+      <c r="I6">
+        <v>600.15099999999995</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" ht="109.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7">
+        <v>600</v>
+      </c>
+      <c r="F7">
+        <v>210931</v>
+      </c>
+      <c r="G7">
+        <v>210931</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>400.7789932</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add solved solution and result table. This project works good enough and it's time to end. Users can directly run main.py for checking only if you processed Gurobi and COPT correctly. It's a nice homework and I have learned a lot. Thanks a lot for the kind help from Prof.Hu.
</commit_message>
<xml_diff>
--- a/tsp结果表头.xlsx
+++ b/tsp结果表头.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NJU\Projects\TSP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA384929-A48F-4B64-BD92-131F257435A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D951DA84-4F71-4962-BA3D-D4C373BC38D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F621E1B-0013-FB40-BA1E-B470E5CCCC83}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="23232" windowHeight="6216" xr2:uid="{1F621E1B-0013-FB40-BA1E-B470E5CCCC83}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,9 @@
   </si>
   <si>
     <t>1. Callback: 只有找到合法子环，才添加lazy constraint把该子环排除；放弃在硬约束中排除所有子环
-2. 参数调优：
+2. 求最短子环的函数不会找到对称子环，以破解对称性
+3.在Gurobi求解之前使用最近邻算法生成初始可行路径，并设置为初始解
+4. 参数调优：
 model.setParam(COPT.Param.HeurLevel, 3)
         model.setParam(COPT.Param.Threads, 8)
         model.setParam(COPT.Param.Presolve, 2)</t>
@@ -523,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9902200E-5C89-164B-9530-850F7BA4D82E}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
@@ -569,7 +571,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="234">
+    <row r="2" spans="1:10" ht="250.95" customHeight="1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -586,7 +588,7 @@
         <v>600</v>
       </c>
       <c r="F2">
-        <v>48834</v>
+        <v>48832</v>
       </c>
       <c r="G2">
         <v>48910</v>
@@ -601,7 +603,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="127.2" customHeight="1">
+    <row r="3" spans="1:10" ht="250.95" customHeight="1">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -618,22 +620,22 @@
         <v>600</v>
       </c>
       <c r="F3">
-        <v>47113</v>
+        <v>47721.110999999997</v>
       </c>
       <c r="G3">
-        <v>47113</v>
+        <v>59714</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>20.083881315749998</v>
       </c>
       <c r="I3">
-        <v>32.058999999999997</v>
+        <v>600.17999999999995</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="234">
+    <row r="4" spans="1:10" ht="250.95" customHeight="1">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -650,22 +652,22 @@
         <v>600</v>
       </c>
       <c r="F4">
-        <v>6771</v>
+        <v>6770</v>
       </c>
       <c r="G4">
         <v>6773</v>
       </c>
       <c r="H4">
-        <v>2.9529012254540001E-2</v>
+        <v>4.4293158300000003E-2</v>
       </c>
       <c r="I4">
-        <v>600.03299999237004</v>
+        <v>600.04200000000003</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="109.2">
+    <row r="5" spans="1:10" ht="250.95" customHeight="1">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -682,22 +684,22 @@
         <v>600</v>
       </c>
       <c r="F5">
-        <v>6685</v>
+        <v>6761</v>
       </c>
       <c r="G5">
-        <v>6685</v>
+        <v>8536</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>20.783193700000002</v>
       </c>
       <c r="I5">
-        <v>26.873998641966999</v>
+        <v>600.33000000000004</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="234">
+    <row r="6" spans="1:10" ht="250.95" customHeight="1">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -723,13 +725,13 @@
         <v>17.74009431967</v>
       </c>
       <c r="I6">
-        <v>600.15099999999995</v>
+        <v>600.09</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="109.2">
+    <row r="7" spans="1:10" ht="250.95" customHeight="1">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -746,16 +748,16 @@
         <v>600</v>
       </c>
       <c r="F7">
-        <v>210931</v>
+        <v>211007.25</v>
       </c>
       <c r="G7">
-        <v>210931</v>
+        <v>305404</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>30.9088125</v>
       </c>
       <c r="I7">
-        <v>400.7789932</v>
+        <v>600.9</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>18</v>

</xml_diff>